<commit_message>
Some phase 1 paper results and scripts
</commit_message>
<xml_diff>
--- a/RandomAccess/results/gups.xlsx
+++ b/RandomAccess/results/gups.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Native</t>
   </si>
@@ -42,13 +42,10 @@
     <t>RAW DATA</t>
   </si>
   <si>
-    <t>Median</t>
+    <t>Mean</t>
   </si>
   <si>
-    <t>Max-Median</t>
-  </si>
-  <si>
-    <t>Median-Min</t>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -103,8 +100,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -127,7 +126,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -135,6 +134,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -142,6 +142,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -196,13 +197,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.002742647</c:v>
+                    <c:v>0.00144049876440191</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.00344742699999999</c:v>
+                    <c:v>0.00187314187556606</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.003177861</c:v>
+                    <c:v>0.00147609522979863</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -214,13 +215,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.001244842</c:v>
+                    <c:v>0.00144049876440191</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.001961725</c:v>
+                    <c:v>0.00187314187556606</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.002061102</c:v>
+                    <c:v>0.00147609522979863</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -250,13 +251,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.045320895</c:v>
+                  <c:v>0.0457918159</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.045310911</c:v>
+                  <c:v>0.0457380556</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.039108695</c:v>
+                  <c:v>0.0393632655</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -271,11 +272,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2134256104"/>
-        <c:axId val="-2134259432"/>
+        <c:axId val="2082641032"/>
+        <c:axId val="2137592696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2134256104"/>
+        <c:axId val="2082641032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,7 +285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134259432"/>
+        <c:crossAx val="2137592696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -292,7 +293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134259432"/>
+        <c:axId val="2137592696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134256104"/>
+        <c:crossAx val="2082641032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -391,13 +392,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.000501394000000002</c:v>
+                    <c:v>0.000285644660726283</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0009806385</c:v>
+                    <c:v>0.000440471497297107</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.000787058999999999</c:v>
+                    <c:v>0.000315264345606456</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -409,13 +410,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.000415919999999998</c:v>
+                    <c:v>0.000285644660726283</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.000455981500000001</c:v>
+                    <c:v>0.000440471497297107</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.000314136000000001</c:v>
+                    <c:v>0.000315264345606456</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -445,13 +446,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.012581883</c:v>
+                  <c:v>0.0126129369</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0122327245</c:v>
+                  <c:v>0.0123961444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.012370234</c:v>
+                  <c:v>0.012475643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,11 +467,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133876776"/>
-        <c:axId val="-2133873800"/>
+        <c:axId val="2137630584"/>
+        <c:axId val="2137666040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133876776"/>
+        <c:axId val="2137630584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133873800"/>
+        <c:crossAx val="2137666040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -487,7 +488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133873800"/>
+        <c:axId val="2137666040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.015"/>
@@ -519,7 +520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133876776"/>
+        <c:crossAx val="2137630584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -930,7 +931,7 @@
   <dimension ref="A16:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:G28"/>
+      <selection activeCell="C29" sqref="C29:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1201,28 +1202,28 @@
         <v>7</v>
       </c>
       <c r="B29" s="1">
-        <f>MEDIAN(B19:B28)</f>
-        <v>4.5320895E-2</v>
+        <f>AVERAGE(B19:B28)</f>
+        <v>4.5791815900000005E-2</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" ref="C29:G29" si="0">MEDIAN(C19:C28)</f>
-        <v>4.5310911000000002E-2</v>
+        <f t="shared" ref="C29:G29" si="0">AVERAGE(C19:C28)</f>
+        <v>4.5738055600000008E-2</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>3.9108694999999999E-2</v>
+        <v>3.9363265500000001E-2</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>1.2581882999999999E-2</v>
+        <v>1.2612936900000002E-2</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>1.22327245E-2</v>
+        <v>1.23961444E-2</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="0"/>
-        <v>1.2370234000000001E-2</v>
+        <v>1.2475643E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
@@ -1230,57 +1231,57 @@
         <v>8</v>
       </c>
       <c r="B30" s="1">
-        <f>MAX(B19:B28)-B29</f>
-        <v>2.7426470000000008E-3</v>
+        <f>STDEV(B19:B28)</f>
+        <v>1.4404987644019119E-3</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" ref="C30:G30" si="1">MAX(C19:C28)-C29</f>
-        <v>3.447426999999996E-3</v>
+        <f t="shared" ref="C30:G30" si="1">STDEV(C19:C28)</f>
+        <v>1.873141875566065E-3</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="1"/>
-        <v>3.177861000000004E-3</v>
+        <v>1.4760952297986339E-3</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="1"/>
-        <v>5.0139400000000223E-4</v>
+        <v>2.8564466072628308E-4</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
-        <v>9.8063850000000043E-4</v>
+        <v>4.4047149729710763E-4</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="1"/>
-        <v>7.8705899999999968E-4</v>
+        <v>3.1526434560645588E-4</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1">
-        <f>B29-MIN(B19:B28)</f>
-        <v>1.2448420000000029E-3</v>
+        <f>STDEV(B19:B28)</f>
+        <v>1.4404987644019119E-3</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:G31" si="2">C29-MIN(C19:C28)</f>
-        <v>1.9617250000000044E-3</v>
+        <f t="shared" ref="C31:G31" si="2">STDEV(C19:C28)</f>
+        <v>1.873141875566065E-3</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="2"/>
-        <v>2.0611020000000022E-3</v>
+        <v>1.4760952297986339E-3</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="2"/>
-        <v>4.1591999999999844E-4</v>
+        <v>2.8564466072628308E-4</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="2"/>
-        <v>4.5598150000000087E-4</v>
+        <v>4.4047149729710763E-4</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="2"/>
-        <v>3.1413600000000132E-4</v>
+        <v>3.1526434560645588E-4</v>
       </c>
     </row>
     <row r="34" spans="2:7">

</xml_diff>